<commit_message>
Reviso actividad tema 2
</commit_message>
<xml_diff>
--- a/docs/T_01_Fundamentos_SO/Actividades/Guia_Evaluacion_Act1.xlsx
+++ b/docs/T_01_Fundamentos_SO/Actividades/Guia_Evaluacion_Act1.xlsx
@@ -225,12 +225,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="49.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="45.91"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="11.54"/>
   </cols>
@@ -340,7 +340,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>